<commit_message>
A bunch of shiet
ye
</commit_message>
<xml_diff>
--- a/VSTOXX_data.xlsx
+++ b/VSTOXX_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13399" uniqueCount="6701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13415" uniqueCount="6709">
   <si>
     <t>07.01.1999</t>
   </si>
@@ -20117,6 +20117,30 @@
   </si>
   <si>
     <t>30.04.2025</t>
+  </si>
+  <si>
+    <t>02.05.2025</t>
+  </si>
+  <si>
+    <t>05.05.2025</t>
+  </si>
+  <si>
+    <t>06.05.2025</t>
+  </si>
+  <si>
+    <t>07.05.2025</t>
+  </si>
+  <si>
+    <t>08.05.2025</t>
+  </si>
+  <si>
+    <t>09.05.2025</t>
+  </si>
+  <si>
+    <t>12.05.2025</t>
+  </si>
+  <si>
+    <t>13.05.2025</t>
   </si>
 </sst>
 </file>
@@ -20474,7 +20498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6699"/>
+  <dimension ref="A1:C6707"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -94169,6 +94193,94 @@
         <v>22.4714</v>
       </c>
     </row>
+    <row r="6700" spans="1:3">
+      <c r="A6700" t="s">
+        <v>6701</v>
+      </c>
+      <c r="B6700" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6700">
+        <v>20.5365</v>
+      </c>
+    </row>
+    <row r="6701" spans="1:3">
+      <c r="A6701" t="s">
+        <v>6702</v>
+      </c>
+      <c r="B6701" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6701">
+        <v>20.2803</v>
+      </c>
+    </row>
+    <row r="6702" spans="1:3">
+      <c r="A6702" t="s">
+        <v>6703</v>
+      </c>
+      <c r="B6702" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6702">
+        <v>20.7876</v>
+      </c>
+    </row>
+    <row r="6703" spans="1:3">
+      <c r="A6703" t="s">
+        <v>6704</v>
+      </c>
+      <c r="B6703" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6703">
+        <v>21.6622</v>
+      </c>
+    </row>
+    <row r="6704" spans="1:3">
+      <c r="A6704" t="s">
+        <v>6705</v>
+      </c>
+      <c r="B6704" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6704">
+        <v>20.4215</v>
+      </c>
+    </row>
+    <row r="6705" spans="1:3">
+      <c r="A6705" t="s">
+        <v>6706</v>
+      </c>
+      <c r="B6705" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6705">
+        <v>20.5188</v>
+      </c>
+    </row>
+    <row r="6706" spans="1:3">
+      <c r="A6706" t="s">
+        <v>6707</v>
+      </c>
+      <c r="B6706" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6706">
+        <v>18.1951</v>
+      </c>
+    </row>
+    <row r="6707" spans="1:3">
+      <c r="A6707" t="s">
+        <v>6708</v>
+      </c>
+      <c r="B6707" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6707">
+        <v>16.5618</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>